<commit_message>
Sheet bundle saved issue
</commit_message>
<xml_diff>
--- a/migration/backend/storage/sheets/0e6354d1-beff-11f0-a49a-00155d07fa06/7b843c49-bfe7-11f0-ad7f-40c2baaf5526/1765856429600-demo_file.xlsx
+++ b/migration/backend/storage/sheets/0e6354d1-beff-11f0-a49a-00155d07fa06/7b843c49-bfe7-11f0-ad7f-40c2baaf5526/1765856429600-demo_file.xlsx
@@ -489,35 +489,35 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="M2" t="str">
-        <v/>
-      </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
-      <c r="O2" t="str">
-        <v/>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
       </c>
       <c r="P2" t="str">
         <v>2403617614921002</v>
@@ -541,7 +541,7 @@
         <v/>
       </c>
       <c r="W2">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">

</xml_diff>